<commit_message>
WIP Version 1.3.0 : programming done, WIP leaktest adding defect code input
</commit_message>
<xml_diff>
--- a/excel_import/programming_report_template.xlsx
+++ b/excel_import/programming_report_template.xlsx
@@ -5,22 +5,35 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://johnsonoutdoorsinc-my.sharepoint.com/personal/david_zhang_johnsonoutdoors_com/Documents/David's Stuff/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://johnsonoutdoorsinc-my.sharepoint.com/personal/david_zhang_johnsonoutdoors_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="190" documentId="13_ncr:1_{A1CECE6E-458F-422C-A05E-4186ECEC6448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBE2D118-4200-41FD-A79E-8FCF90080AD5}"/>
+  <xr:revisionPtr revIDLastSave="204" documentId="13_ncr:1_{A1CECE6E-458F-422C-A05E-4186ECEC6448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1DBB4DB-E465-46BA-950C-4D1F9A110B19}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Programming Result Report</t>
   </si>
@@ -40,24 +53,6 @@
     <t>Result</t>
   </si>
   <si>
-    <t>fail_current</t>
-  </si>
-  <si>
-    <t>fail_hr</t>
-  </si>
-  <si>
-    <t>fail_pairing</t>
-  </si>
-  <si>
-    <t>fail_bluetooth</t>
-  </si>
-  <si>
-    <t>fail_sleep_mode</t>
-  </si>
-  <si>
-    <t>fail_other</t>
-  </si>
-  <si>
     <t>Date Created</t>
   </si>
   <si>
@@ -77,6 +72,12 @@
   </si>
   <si>
     <t>Generated By :</t>
+  </si>
+  <si>
+    <t>Error Code</t>
+  </si>
+  <si>
+    <t>Error Description</t>
   </si>
 </sst>
 </file>
@@ -567,31 +568,27 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M11"/>
+  <dimension ref="B1:I11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" style="13" customWidth="1"/>
     <col min="2" max="3" width="22.42578125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="13" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" style="11" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="11" customWidth="1"/>
-    <col min="12" max="12" width="18" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" style="12" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="13" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="13"/>
+    <col min="6" max="6" width="11.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.42578125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="18" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="12" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" s="1" customFormat="1" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" s="1" customFormat="1" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="4"/>
       <c r="C1" s="14"/>
       <c r="D1" s="4"/>
@@ -599,13 +596,9 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="8"/>
-    </row>
-    <row r="2" spans="2:13" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="2:9" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -614,38 +607,30 @@
       </c>
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="2:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="5"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" s="19"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="8"/>
-    </row>
-    <row r="4" spans="2:13" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="16"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="2:9" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="3"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="8"/>
-    </row>
-    <row r="5" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="16"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="2:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
         <v>1</v>
       </c>
@@ -654,14 +639,12 @@
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="2"/>
-      <c r="L5" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="19"/>
-    </row>
-    <row r="6" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="2:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
         <v>2</v>
       </c>
@@ -670,14 +653,12 @@
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="2"/>
-      <c r="L6" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" s="19"/>
-    </row>
-    <row r="7" spans="2:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H6" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="2:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -685,18 +666,14 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="2:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>4</v>
@@ -705,48 +682,36 @@
         <v>5</v>
       </c>
       <c r="F8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" s="18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="E2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="67" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Version 1.4.0 : Completed
</commit_message>
<xml_diff>
--- a/excel_import/programming_report_template.xlsx
+++ b/excel_import/programming_report_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://johnsonoutdoorsinc-my.sharepoint.com/personal/david_zhang_johnsonoutdoors_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="204" documentId="13_ncr:1_{A1CECE6E-458F-422C-A05E-4186ECEC6448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1DBB4DB-E465-46BA-950C-4D1F9A110B19}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="13_ncr:1_{A1CECE6E-458F-422C-A05E-4186ECEC6448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C097D54A-A582-4560-94DD-763A85C390F5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Programming Result Report</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Error Description</t>
+  </si>
+  <si>
+    <t>Lot No.</t>
+  </si>
+  <si>
+    <t>Remarks</t>
   </si>
 </sst>
 </file>
@@ -189,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -247,6 +253,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -568,69 +577,77 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I11"/>
+  <dimension ref="B1:K11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" style="13" customWidth="1"/>
     <col min="2" max="3" width="22.42578125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="16" style="13" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.42578125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="18" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="12" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="13" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="13"/>
+    <col min="4" max="4" width="17.85546875" style="13" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.42578125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="18" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="12" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="13" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="1" customFormat="1" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" s="1" customFormat="1" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="4"/>
       <c r="C1" s="14"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="2"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="8"/>
-    </row>
-    <row r="2" spans="2:9" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="2:11" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="9"/>
-    </row>
-    <row r="3" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="19"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="2:9" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="16"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="2:11" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="2:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="2:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
         <v>1</v>
       </c>
@@ -639,12 +656,14 @@
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="19"/>
-    </row>
-    <row r="6" spans="2:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="19"/>
+    </row>
+    <row r="6" spans="2:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
         <v>2</v>
       </c>
@@ -653,22 +672,26 @@
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="19"/>
-    </row>
-    <row r="7" spans="2:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K6" s="19"/>
+    </row>
+    <row r="7" spans="2:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="14"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="2:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="2:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>3</v>
       </c>
@@ -678,40 +701,49 @@
       <c r="D8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="G8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="H8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="I8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="K8" s="18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="F2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="67" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>